<commit_message>
updated 1990-1998 of newbuilding and secondhand with Lloyd shipping Economist data
</commit_message>
<xml_diff>
--- a/input/Lloyd_shipping_economist_1980_1998.xlsx
+++ b/input/Lloyd_shipping_economist_1980_1998.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sugur\Dropbox\ship\containerfreightrate\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sugur\Dropbox\ship\container_data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6256A0-18C3-4076-A71B-402C05377928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C2330DB-624E-4446-90B2-7F3299444EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="3330" windowWidth="17760" windowHeight="11055" xr2:uid="{7E79088B-8FE4-4801-A8AF-3E950BE07E9B}"/>
+    <workbookView xWindow="60" yWindow="3510" windowWidth="17760" windowHeight="11055" xr2:uid="{7E79088B-8FE4-4801-A8AF-3E950BE07E9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
   <si>
     <t>year</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>current_dollars</t>
+  </si>
+  <si>
+    <t>newbuilding_price_per_dwt_2500teu_fullcon</t>
   </si>
 </sst>
 </file>
@@ -547,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93644C77-C033-4777-AF82-0D86742AC273}">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -728,7 +731,7 @@
         <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E10">
         <v>859</v>
@@ -745,7 +748,7 @@
         <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E11">
         <v>1205</v>
@@ -762,7 +765,7 @@
         <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <v>1321</v>
@@ -779,9 +782,11 @@
         <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1616</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14">
@@ -794,9 +799,11 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1282</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15">
@@ -809,9 +816,11 @@
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
-      </c>
-      <c r="E15" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1205</v>
+      </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16">
@@ -824,9 +833,11 @@
         <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1077</v>
+      </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17">
@@ -839,9 +850,11 @@
         <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E17" s="1">
+        <v>2000</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18">
@@ -854,9 +867,11 @@
         <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1800</v>
+      </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
@@ -869,9 +884,11 @@
         <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1800</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
@@ -884,9 +901,11 @@
         <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1150</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21">
@@ -1088,7 +1107,9 @@
       <c r="D32" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="1"/>
+      <c r="E32" s="1">
+        <v>865</v>
+      </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33">
@@ -1103,7 +1124,9 @@
       <c r="D33" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="1">
+        <v>816</v>
+      </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34">
@@ -1118,7 +1141,9 @@
       <c r="D34" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="1"/>
+      <c r="E34" s="1">
+        <v>790</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35">
@@ -1133,7 +1158,9 @@
       <c r="D35" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="1"/>
+      <c r="E35" s="1">
+        <v>827</v>
+      </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36">
@@ -1148,7 +1175,9 @@
       <c r="D36" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="1"/>
+      <c r="E36" s="1">
+        <v>977</v>
+      </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37">
@@ -1163,7 +1192,9 @@
       <c r="D37" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="1"/>
+      <c r="E37" s="1">
+        <v>977</v>
+      </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38">
@@ -1178,7 +1209,9 @@
       <c r="D38" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="1"/>
+      <c r="E38" s="1">
+        <v>977</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39">
@@ -1193,7 +1226,9 @@
       <c r="D39" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="1"/>
+      <c r="E39" s="1">
+        <v>751</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>